<commit_message>
Updates to data munging
</commit_message>
<xml_diff>
--- a/2017/Spring2017Datasheet.xlsx
+++ b/2017/Spring2017Datasheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebatzer\Box Sync\Eviner lab shared\Evan\Research Projects\Spatial Scaling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebatzer\Box Sync\Eviner lab shared\Evan\Research Projects\Spatial-Scaling\2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -625,7 +625,7 @@
   <dimension ref="A1:AI80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AX69" sqref="AX69"/>
+      <selection activeCell="BB63" sqref="BB63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.375" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>